<commit_message>
day 5  attandance marked
</commit_message>
<xml_diff>
--- a/student list.xlsx
+++ b/student list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\internship\PPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\internship\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EE488D-F94C-4225-AA45-8B8AF51E4094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F16776-C40D-412B-BDDA-40F0A644EB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="271" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="271" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1 " sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="33">
   <si>
     <t>Sr No.</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Adhiraj Kate</t>
+  </si>
+  <si>
+    <t>Web Devlopment Internship 2024 (Week 2)</t>
   </si>
 </sst>
 </file>
@@ -396,6 +399,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -413,9 +419,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -699,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E24" sqref="B2:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,15 +714,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
@@ -1107,7 +1110,7 @@
       <c r="F23" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="28"/>
+      <c r="G23" s="22"/>
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
@@ -1157,12 +1160,367 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C9C37C-F6D8-4B8C-8D27-CA08E1AF3E8D}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+    </row>
+    <row r="3" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45453</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="17">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="16">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="17">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="16">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="17">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="16">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="17">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="16">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="17">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="16">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="17">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="16">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="17">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="16">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="17">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="16">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="17">
+        <v>18</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="16">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="17">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="19"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="16">
+        <v>21</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="15">
+        <v>22</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1179,24 +1537,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="2:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="27"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="4" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
day 6 intorduction to bootstrap
</commit_message>
<xml_diff>
--- a/student list.xlsx
+++ b/student list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\internship\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F16776-C40D-412B-BDDA-40F0A644EB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF47220-3AB7-497E-A95E-24B33AFBC0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="271" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="33">
   <si>
     <t>Sr No.</t>
   </si>
@@ -1162,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C9C37C-F6D8-4B8C-8D27-CA08E1AF3E8D}">
   <dimension ref="B2:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,7 +1192,9 @@
       <c r="D3" s="4">
         <v>45453</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4">
+        <v>45454</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
@@ -1209,7 +1211,9 @@
       <c r="D4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F4" s="14"/>
       <c r="G4" s="16"/>
       <c r="H4" s="1"/>
@@ -1224,7 +1228,9 @@
       <c r="D5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="F5" s="15"/>
       <c r="G5" s="17"/>
       <c r="H5" s="2"/>
@@ -1239,7 +1245,9 @@
       <c r="D6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F6" s="14"/>
       <c r="G6" s="16"/>
       <c r="H6" s="1"/>
@@ -1267,7 +1275,9 @@
       <c r="D8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F8" s="14"/>
       <c r="G8" s="16"/>
       <c r="H8" s="1"/>
@@ -1282,7 +1292,9 @@
       <c r="D9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="F9" s="15"/>
       <c r="G9" s="17"/>
       <c r="H9" s="2"/>
@@ -1295,7 +1307,9 @@
         <v>9</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F10" s="14"/>
       <c r="G10" s="16"/>
       <c r="H10" s="1"/>
@@ -1325,7 +1339,9 @@
       <c r="D12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F12" s="14"/>
       <c r="G12" s="16"/>
       <c r="H12" s="1"/>
@@ -1340,7 +1356,9 @@
       <c r="D13" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="15"/>
+      <c r="E13" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="F13" s="15"/>
       <c r="G13" s="17"/>
       <c r="H13" s="2"/>
@@ -1353,7 +1371,9 @@
         <v>13</v>
       </c>
       <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
+      <c r="E14" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F14" s="14"/>
       <c r="G14" s="16"/>
       <c r="H14" s="1"/>
@@ -1396,7 +1416,9 @@
       <c r="D17" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="15"/>
+      <c r="E17" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="F17" s="15"/>
       <c r="G17" s="17"/>
       <c r="H17" s="2"/>
@@ -1409,7 +1431,9 @@
         <v>17</v>
       </c>
       <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="E18" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F18" s="14"/>
       <c r="G18" s="16"/>
       <c r="H18" s="1"/>
@@ -1452,7 +1476,9 @@
       <c r="D21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="15"/>
+      <c r="E21" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="F21" s="15"/>
       <c r="G21" s="17"/>
       <c r="H21" s="2"/>
@@ -1467,7 +1493,9 @@
       <c r="D22" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F22" s="14"/>
       <c r="G22" s="16"/>
       <c r="H22" s="1"/>
@@ -1482,7 +1510,9 @@
       <c r="D23" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="F23" s="18"/>
       <c r="G23" s="22"/>
       <c r="H23" s="19"/>
@@ -1497,7 +1527,9 @@
       <c r="D24" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="F24" s="14"/>
       <c r="G24" s="16"/>
       <c r="H24" s="1"/>
@@ -1512,7 +1544,9 @@
       <c r="D25" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="15"/>
+      <c r="E25" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>

</xml_diff>

<commit_message>
day 9 java script
</commit_message>
<xml_diff>
--- a/student list.xlsx
+++ b/student list.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\internship\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C9D435-703E-4E98-AD16-5E71DC8BB942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F75D7EE-F9F4-4971-A51E-4F09E1C079BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="271" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="271" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1 " sheetId="1" r:id="rId1"/>
     <sheet name="Week 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Assignment" sheetId="3" r:id="rId3"/>
+    <sheet name="Week 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Assignment" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="34">
   <si>
     <t>Sr No.</t>
   </si>
@@ -126,6 +127,9 @@
   </si>
   <si>
     <t>Web Devlopment Internship 2024 (Week 2)</t>
+  </si>
+  <si>
+    <t>Web Devlopment Internship 2024 (Week 3)</t>
   </si>
 </sst>
 </file>
@@ -1162,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C9C37C-F6D8-4B8C-8D27-CA08E1AF3E8D}">
   <dimension ref="B2:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,6 +1626,377 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3826BB-7596-4565-8433-FC05CF46CABA}">
+  <dimension ref="B3:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45462</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="17">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="16">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="17">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="16">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="17">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="17">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="16">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="17">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="16">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="17">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="16">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="17">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="16">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="17">
+        <v>16</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="16">
+        <v>17</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="17">
+        <v>18</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="16">
+        <v>19</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="17">
+        <v>20</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="16">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="15">
+        <v>22</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0895A4BE-6540-4277-ACAB-EFBA1C9CB06B}">
   <dimension ref="B1:H22"/>
   <sheetViews>

</xml_diff>

<commit_message>
day 11 code uploaded
</commit_message>
<xml_diff>
--- a/student list.xlsx
+++ b/student list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\internship\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66AB341-6C8D-40CB-8C67-A99E1E689D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C863C419-3697-4191-8E9E-FB98434B5F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="271" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="34">
   <si>
     <t>Sr No.</t>
   </si>
@@ -1630,7 +1630,7 @@
   <dimension ref="B3:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1662,7 +1662,9 @@
       <c r="E4" s="4">
         <v>45463</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4">
+        <v>45464</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="3" t="s">
         <v>22</v>
@@ -1679,7 +1681,9 @@
         <v>28</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="F5" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="G5" s="16"/>
       <c r="H5" s="1"/>
     </row>
@@ -1696,7 +1700,9 @@
       <c r="E6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="G6" s="17"/>
       <c r="H6" s="2"/>
     </row>
@@ -1730,7 +1736,9 @@
       <c r="E8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="G8" s="17"/>
       <c r="H8" s="2"/>
     </row>
@@ -1747,7 +1755,9 @@
       <c r="E9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="G9" s="16"/>
       <c r="H9" s="1"/>
     </row>
@@ -1764,7 +1774,9 @@
       <c r="E10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="15"/>
+      <c r="F10" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="G10" s="17"/>
       <c r="H10" s="2"/>
     </row>
@@ -1843,7 +1855,9 @@
       <c r="E15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="G15" s="16"/>
       <c r="H15" s="1"/>
     </row>
@@ -1860,7 +1874,9 @@
       <c r="E16" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="G16" s="17"/>
       <c r="H16" s="2"/>
     </row>
@@ -1875,7 +1891,9 @@
         <v>28</v>
       </c>
       <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="F17" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="G17" s="16"/>
       <c r="H17" s="1"/>
     </row>
@@ -1892,7 +1910,9 @@
       <c r="E18" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="15"/>
+      <c r="F18" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="G18" s="17"/>
       <c r="H18" s="2"/>
     </row>
@@ -1909,7 +1929,9 @@
       <c r="E19" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="14"/>
+      <c r="F19" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="G19" s="16"/>
       <c r="H19" s="1"/>
     </row>
@@ -1943,7 +1965,9 @@
       <c r="E21" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="14"/>
+      <c r="F21" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="G21" s="16"/>
       <c r="H21" s="1"/>
     </row>
@@ -1977,7 +2001,9 @@
       <c r="E23" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="14"/>
+      <c r="F23" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="G23" s="16"/>
       <c r="H23" s="1"/>
     </row>
@@ -2007,7 +2033,9 @@
       <c r="E25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="14"/>
+      <c r="F25" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="G25" s="16"/>
       <c r="H25" s="1"/>
     </row>

</xml_diff>

<commit_message>
day 13 and Calculater project
</commit_message>
<xml_diff>
--- a/student list.xlsx
+++ b/student list.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\internship\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FFC2B4-9171-4CFC-A1F9-842C34261F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AA88B8-742B-4330-894C-24F7CB2B1305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="271" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="271" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1 " sheetId="1" r:id="rId1"/>
     <sheet name="Week 2" sheetId="2" r:id="rId2"/>
     <sheet name="Week 3" sheetId="4" r:id="rId3"/>
-    <sheet name="Assignment" sheetId="3" r:id="rId4"/>
+    <sheet name="Week 4" sheetId="5" r:id="rId4"/>
+    <sheet name="Assignment" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="35">
   <si>
     <t>Sr No.</t>
   </si>
@@ -1632,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3826BB-7596-4565-8433-FC05CF46CABA}">
   <dimension ref="B3:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C11" sqref="B3:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2102,6 +2103,379 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFC06FD-233F-4592-8000-96F5ED07DA80}">
+  <dimension ref="B3:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45468</v>
+      </c>
+      <c r="E4" s="4">
+        <v>45469</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45470</v>
+      </c>
+      <c r="G4" s="4">
+        <v>45471</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="17">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="16">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="17">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="16">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="17">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="17">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="16">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="17">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="16">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="17">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="16">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="17">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="16">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="17">
+        <v>16</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="16">
+        <v>17</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="17">
+        <v>18</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="16">
+        <v>19</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="17">
+        <v>20</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="16">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="15">
+        <v>22</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0895A4BE-6540-4277-ACAB-EFBA1C9CB06B}">
   <dimension ref="B1:H22"/>
   <sheetViews>

</xml_diff>